<commit_message>
finishing up the Change Log Translation program
</commit_message>
<xml_diff>
--- a/Campaign.xlsx
+++ b/Campaign.xlsx
@@ -14,7 +14,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>TEST TWO</t>
+  </si>
+  <si>
+    <t>TEST ONE</t>
+  </si>
+  <si>
+    <t>TEST THREE</t>
+  </si>
   <si>
     <t>2018»Italy»BG-GMC-Truck-Retail-NC»GMC-Truck-Full-Line(Hispanic)»Regional»In-Market»84671329651657</t>
   </si>
@@ -370,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -378,7 +387,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -404,6 +413,21 @@
     <row r="6" spans="1:1">
       <c r="A6" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
6/5/2018 7:19PM completed changeLogTranslation script. testing begins tomorrow morning. Also wrote a quick script for the 404 error report
</commit_message>
<xml_diff>
--- a/Campaign.xlsx
+++ b/Campaign.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>TEST TWO</t>
   </si>
@@ -26,18 +26,6 @@
   </si>
   <si>
     <t>2018»Italy»BG-GMC-Truck-Retail-NC»GMC-Truck-Full-Line(Hispanic)»Regional»In-Market»84671329651657</t>
-  </si>
-  <si>
-    <t>banana»kale»hawk»antelope»thor»superman</t>
-  </si>
-  <si>
-    <t>grape»artichoke»sparrow»bear»black panther»aquaman</t>
-  </si>
-  <si>
-    <t>apple»carrot»robin»hamster»spider-man»batman</t>
-  </si>
-  <si>
-    <t>SWHITE TESTING PLEASE DELETE</t>
   </si>
   <si>
     <t>Campaign Name</t>
@@ -379,7 +367,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -387,7 +375,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -410,26 +398,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Forgot to upload latest updates from yesterday 6/6/2018. 6/7/2018 12:35PM uploading recent changes. nothing too major in this update. need to do more testing, and starting a request module for DBM stuff
</commit_message>
<xml_diff>
--- a/Campaign.xlsx
+++ b/Campaign.xlsx
@@ -14,7 +14,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>apple»SUCCESS»Test»TEST»TEST»TEST»TEST</t>
+  </si>
+  <si>
+    <t>apple»carrot»robin»TEST»TEST»TEST»TEST</t>
+  </si>
+  <si>
+    <t>grape»artichoke»sparrow»bear»TEST»TEST</t>
+  </si>
+  <si>
+    <t>banana»kale»hawk»antelope»thor»TEST»TEST</t>
+  </si>
+  <si>
+    <t>apple»carrot»robin»hamster»spider-man»TEST»TEST</t>
+  </si>
+  <si>
+    <t>apple»carrot»robin»hamster»spider-man»batman»TEST</t>
+  </si>
+  <si>
+    <t>banana»kale»hawk»antelope»thor»superman»TEST</t>
+  </si>
+  <si>
+    <t>grape»artichoke»sparrow»bear»black panther»TEST</t>
+  </si>
+  <si>
+    <t>TEST Five</t>
+  </si>
+  <si>
+    <t>TEST Four</t>
+  </si>
   <si>
     <t>TEST TWO</t>
   </si>
@@ -23,9 +53,6 @@
   </si>
   <si>
     <t>TEST THREE</t>
-  </si>
-  <si>
-    <t>2018»Italy»BG-GMC-Truck-Retail-NC»GMC-Truck-Full-Line(Hispanic)»Regional»In-Market»84671329651657</t>
   </si>
   <si>
     <t>Campaign Name</t>
@@ -367,7 +394,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -375,7 +402,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -396,6 +423,51 @@
     <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All current Commits for 7/5/2018
</commit_message>
<xml_diff>
--- a/Campaign.xlsx
+++ b/Campaign.xlsx
@@ -14,45 +14,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>apple»SUCCESS»Test»TEST»TEST»TEST»TEST</t>
-  </si>
-  <si>
-    <t>apple»carrot»robin»TEST»TEST»TEST»TEST</t>
-  </si>
-  <si>
-    <t>grape»artichoke»sparrow»bear»TEST»TEST</t>
-  </si>
-  <si>
-    <t>banana»kale»hawk»antelope»thor»TEST»TEST</t>
-  </si>
-  <si>
-    <t>apple»carrot»robin»hamster»spider-man»TEST»TEST</t>
-  </si>
-  <si>
-    <t>apple»carrot»robin»hamster»spider-man»batman»TEST</t>
-  </si>
-  <si>
-    <t>banana»kale»hawk»antelope»thor»superman»TEST</t>
-  </si>
-  <si>
-    <t>grape»artichoke»sparrow»bear»black panther»TEST</t>
-  </si>
-  <si>
-    <t>TEST Five</t>
-  </si>
-  <si>
-    <t>TEST Four</t>
-  </si>
-  <si>
-    <t>TEST TWO</t>
-  </si>
-  <si>
-    <t>TEST ONE</t>
-  </si>
-  <si>
-    <t>TEST THREE</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+  <si>
+    <t>apple»artichoke»apple»carrot»carrot»robin»hamster»robin»hamster»robin»thor»hamster»hamster</t>
+  </si>
+  <si>
+    <t>grape»artichoke»grape»artichoke»artichoke»robin»hamster»robin»hamster»robin»thor»hamster»hamster</t>
+  </si>
+  <si>
+    <t>apple»carrot»apple»carrot»carrot»robin»hamster»robin»antelope»robin»thor»hamster»hamster</t>
+  </si>
+  <si>
+    <t>grape»artichoke»grape»artichoke»carrot»robin»hamster»robin»hamster»robin»thor»hamster»hamster</t>
+  </si>
+  <si>
+    <t>grape»artichoke»grape»carrot»carrot»robin»hamster»robin»hamster»robin»thor»hamster»hamster</t>
+  </si>
+  <si>
+    <t>apple»carrot»banana»carrot»carrot»hawk»hamster»hawk»hamster»robin»spider-man»antelope»antelope</t>
+  </si>
+  <si>
+    <t>grape»artichoke»apple»carrot»carrot»robin»hamster»robin»hamster»robin»thor»hamster»hamster</t>
+  </si>
+  <si>
+    <t>grape»carrot»apple»carrot»carrot»robin»hamster»robin»hamster»robin»thor»hamster»hamster</t>
+  </si>
+  <si>
+    <t>banana»carrot»apple»carrot»carrot»robin»hamster»robin»hamster»robin»thor»hamster»hamster</t>
+  </si>
+  <si>
+    <t>apple»carrot»apple»carrot»carrot»robin»hamster»robin»hamster»robin»thor»hamster»hamster</t>
+  </si>
+  <si>
+    <t>CV4/CFH/683_Chevrolet Retail SC _Chevy Full Line HA_Austin Hispanic Regional Plan_BPR_SCR_GNM_2018</t>
+  </si>
+  <si>
+    <t>1LM/PRO/683_Chevy North East LMA_PROVIDENCE / NEW BEDFORD_Q2 LMA_BCN_NER_GNM_2018</t>
+  </si>
+  <si>
+    <t>apple»carrot»banana»kale»kale»robin»antelope»hawk»hamster»hawk»spider-man»antelope»antelope</t>
+  </si>
+  <si>
+    <t>apple»carrot»banana»kale»kale»hawk»antelope»hawk»antelope»hawk»spider-man»antelope»antelope</t>
   </si>
   <si>
     <t>Campaign Name</t>
@@ -394,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,7 +405,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -468,6 +471,11 @@
     <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Haven't committed in a while
</commit_message>
<xml_diff>
--- a/Campaign.xlsx
+++ b/Campaign.xlsx
@@ -14,48 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>apple»artichoke»apple»carrot»carrot»robin»hamster»robin»hamster»robin»thor»hamster»hamster</t>
-  </si>
-  <si>
-    <t>grape»artichoke»grape»artichoke»artichoke»robin»hamster»robin»hamster»robin»thor»hamster»hamster</t>
-  </si>
-  <si>
-    <t>apple»carrot»apple»carrot»carrot»robin»hamster»robin»antelope»robin»thor»hamster»hamster</t>
-  </si>
-  <si>
-    <t>grape»artichoke»grape»artichoke»carrot»robin»hamster»robin»hamster»robin»thor»hamster»hamster</t>
-  </si>
-  <si>
-    <t>grape»artichoke»grape»carrot»carrot»robin»hamster»robin»hamster»robin»thor»hamster»hamster</t>
-  </si>
-  <si>
-    <t>apple»carrot»banana»carrot»carrot»hawk»hamster»hawk»hamster»robin»spider-man»antelope»antelope</t>
-  </si>
-  <si>
-    <t>grape»artichoke»apple»carrot»carrot»robin»hamster»robin»hamster»robin»thor»hamster»hamster</t>
-  </si>
-  <si>
-    <t>grape»carrot»apple»carrot»carrot»robin»hamster»robin»hamster»robin»thor»hamster»hamster</t>
-  </si>
-  <si>
-    <t>banana»carrot»apple»carrot»carrot»robin»hamster»robin»hamster»robin»thor»hamster»hamster</t>
-  </si>
-  <si>
-    <t>apple»carrot»apple»carrot»carrot»robin»hamster»robin»hamster»robin»thor»hamster»hamster</t>
-  </si>
-  <si>
-    <t>CV4/CFH/683_Chevrolet Retail SC _Chevy Full Line HA_Austin Hispanic Regional Plan_BPR_SCR_GNM_2018</t>
-  </si>
-  <si>
-    <t>1LM/PRO/683_Chevy North East LMA_PROVIDENCE / NEW BEDFORD_Q2 LMA_BCN_NER_GNM_2018</t>
-  </si>
-  <si>
-    <t>apple»carrot»banana»kale»kale»robin»antelope»hawk»hamster»hawk»spider-man»antelope»antelope</t>
-  </si>
-  <si>
-    <t>apple»carrot»banana»kale»kale»hawk»antelope»hawk»antelope»hawk»spider-man»antelope»antelope</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>1LM/HAR/701_Chevy North East LMA_HARTFORD-NEW HAVEN_LMA_BCN_NER_GNM_2018</t>
+  </si>
+  <si>
+    <t>UMM/UM/683_Maven_Maven_Peer_BCN_USA_GNM_2018</t>
+  </si>
+  <si>
+    <t>BUN/BD/686_Buick Division_Buick Brand_3Q'18 OLV Digital Video_BLA_USA_GNM_2018_Buick_SPORTS_STREAM</t>
+  </si>
+  <si>
+    <t>BUN/BD/686_Buick Division_Buick Nat'l Full Line_2018 CBS College Football Live Streaming_BPR_USA_GNM_2018</t>
+  </si>
+  <si>
+    <t>CVN/CEA/683_Chevrolet Division_Chevy Equinox AA_Equinox AA_DTU Amplification_AWR_USA_AAM_2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAX/DM/683_Cadillac Division_Cadillac Brand_Variety_BLA_USA_GNM_2018							</t>
   </si>
   <si>
     <t>Campaign Name</t>
@@ -397,7 +373,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -405,7 +381,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -436,46 +412,6 @@
     <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>